<commit_message>
Updated the example with using choose/char function and added conditional formating
</commit_message>
<xml_diff>
--- a/01-Excel/2/Activities/04-Stu_GradeBook/Solved/GradeBook_Solved.xlsx
+++ b/01-Excel/2/Activities/04-Stu_GradeBook/Solved/GradeBook_Solved.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\2\Activities\04-Stu_GradeBook\Solved\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nimidevanggandhi/Desktop/Trilogy/gt-atl-data-pt-03-2020-u-c/01-Excel/2/Activities/04-Stu_GradeBook/Solved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="BF1A678AD42F33819DD9436ADDB833C5BE9FFB50" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{BDDB190D-A0F6-48B1-B36E-906252DB0770}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00F97F7-1CB2-9847-8A50-E7D19786FDB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="20760" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Student Name</t>
   </si>
@@ -127,13 +135,19 @@
   </si>
   <si>
     <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Choice statement base</t>
+  </si>
+  <si>
+    <t>Using Char</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,12 +202,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -219,8 +296,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{5CCE5C80-5AD7-4B5C-B330-B953A54A71A5}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -531,18 +608,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,8 +646,14 @@
       <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -596,8 +681,16 @@
         <f>IF(F2&gt;=90,"A",IF(F2&gt;=80,"B",IF(F2&gt;=70,"C",IF(F2&gt;=60,"D",IF(F2&lt;60,"F")))))</f>
         <v>C</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I2" t="str">
+        <f>CHOOSE(MIN(MAX(_xlfn.FLOOR.MATH(F2/10)-4,1),5),"F","D","C","B","A")</f>
+        <v>C</v>
+      </c>
+      <c r="J2" t="str">
+        <f>CHAR(MIN(MAX(ROUND((10-_xlfn.FLOOR.MATH(F2/10))*1.1,0),1),6)+64)</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -625,8 +718,16 @@
         <f t="shared" ref="H3:H25" si="2">IF(F3&gt;=90,"A",IF(F3&gt;=80,"B",IF(F3&gt;=70,"C",IF(F3&gt;=60,"D",IF(F3&lt;60,"F")))))</f>
         <v>C</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I25" si="3">CHOOSE(MIN(MAX(_xlfn.FLOOR.MATH(F3/10)-4,1),5),"F","D","C","B","A")</f>
+        <v>C</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J25" si="4">CHAR(MIN(MAX(ROUND((10-_xlfn.FLOOR.MATH(F3/10))*1.1,0),1),6)+64)</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -654,8 +755,16 @@
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I4" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="4"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -683,8 +792,16 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I5" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -712,8 +829,16 @@
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I6" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -741,8 +866,16 @@
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I7" t="str">
+        <f t="shared" si="3"/>
+        <v>C</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="4"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -770,8 +903,16 @@
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I8" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -799,8 +940,16 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -828,8 +977,16 @@
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I10" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="4"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -857,8 +1014,16 @@
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I11" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -886,8 +1051,16 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I12" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -915,8 +1088,16 @@
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I13" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -944,8 +1125,16 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I14" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -973,8 +1162,16 @@
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I15" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1002,8 +1199,16 @@
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I16" t="str">
+        <f t="shared" si="3"/>
+        <v>C</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="4"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1031,8 +1236,16 @@
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I17" t="str">
+        <f t="shared" si="3"/>
+        <v>C</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="4"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1060,8 +1273,16 @@
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I18" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="4"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1089,8 +1310,16 @@
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I19" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1118,8 +1347,16 @@
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I20" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1147,8 +1384,16 @@
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I21" t="str">
+        <f t="shared" si="3"/>
+        <v>C</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="4"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1176,8 +1421,16 @@
         <f t="shared" si="2"/>
         <v>A</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I22" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="4"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1205,8 +1458,16 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I23" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1234,8 +1495,16 @@
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I24" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1263,8 +1532,30 @@
         <f t="shared" si="2"/>
         <v>D</v>
       </c>
+      <c r="I25" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="4"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:J25">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$G1="FAIL"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$G1="PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>